<commit_message>
Chapter 2 stuff added
</commit_message>
<xml_diff>
--- a/The Report/Requirements specification.xlsx
+++ b/The Report/Requirements specification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kidic\Documents\Computer Science\Project Work\The Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBBA773-0D38-469C-8B8B-91DD8EB38C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4B9AC4-EF4C-4644-8B27-594D268AE74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="82">
   <si>
     <t>Requirement</t>
   </si>
@@ -39,15 +39,9 @@
     <t>Evidence</t>
   </si>
   <si>
-    <t>Justification</t>
-  </si>
-  <si>
     <t>Success Criteria</t>
   </si>
   <si>
-    <t>Example Solution</t>
-  </si>
-  <si>
     <t>Problem</t>
   </si>
   <si>
@@ -69,17 +63,230 @@
     <t>Subrequirement</t>
   </si>
   <si>
-    <t>i.1</t>
+    <t>Justification/Limitation</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>I.XX</t>
+  </si>
+  <si>
+    <t>WB.XX</t>
+  </si>
+  <si>
+    <t>PS.XX</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Proposed Solution</t>
+  </si>
+  <si>
+    <t>Digital Pantry</t>
+  </si>
+  <si>
+    <t>Item Storage</t>
+  </si>
+  <si>
+    <t>Variant Optionality</t>
+  </si>
+  <si>
+    <t>Storage Specifications</t>
+  </si>
+  <si>
+    <t>Pantry Appendability</t>
+  </si>
+  <si>
+    <t>Pantry GUI</t>
+  </si>
+  <si>
+    <t>Pantry Ingredient Availability</t>
+  </si>
+  <si>
+    <t>Spiciness Tracker</t>
+  </si>
+  <si>
+    <t>Allergy Tracker</t>
+  </si>
+  <si>
+    <t>Food Group Tracker</t>
+  </si>
+  <si>
+    <t>Texture Tracker</t>
+  </si>
+  <si>
+    <t>Amounts Tracker</t>
+  </si>
+  <si>
+    <t>Expiration Detailer</t>
+  </si>
+  <si>
+    <t>Taste Tracker</t>
+  </si>
+  <si>
+    <t>Digital Methodology List</t>
+  </si>
+  <si>
+    <t>Recipe Leftoverability</t>
+  </si>
+  <si>
+    <t>Recipe Methodological Requirements</t>
+  </si>
+  <si>
+    <t>Cuisine Tracker</t>
+  </si>
+  <si>
+    <t>Method List "Quality" Tracker</t>
+  </si>
+  <si>
+    <t>Methodology List GUI</t>
+  </si>
+  <si>
+    <t>Methodology List Appendability</t>
+  </si>
+  <si>
+    <t>PS.1</t>
+  </si>
+  <si>
+    <t>PS.2</t>
+  </si>
+  <si>
+    <t>PS.3</t>
+  </si>
+  <si>
+    <t>Weekly Planner</t>
+  </si>
+  <si>
+    <t>Settings Store Availability</t>
+  </si>
+  <si>
+    <t>Settings Allergies</t>
+  </si>
+  <si>
+    <t>Settings Four Strength Preferences</t>
+  </si>
+  <si>
+    <t>Algorythim</t>
+  </si>
+  <si>
+    <t>Scheduling Meal Time Slots</t>
+  </si>
+  <si>
+    <t>7 Day Current Memory</t>
+  </si>
+  <si>
+    <t>28 Day Previous Memory</t>
+  </si>
+  <si>
+    <t>Meal Factorisation</t>
+  </si>
+  <si>
+    <t>Pantry Look Up Shopping List</t>
+  </si>
+  <si>
+    <t>Pantry Look Up Expiry Dates</t>
+  </si>
+  <si>
+    <t>PS.1.1</t>
+  </si>
+  <si>
+    <t>PS.1.2</t>
+  </si>
+  <si>
+    <t>PS.1.3</t>
+  </si>
+  <si>
+    <t>PS.1.4</t>
+  </si>
+  <si>
+    <t>PS.1.5</t>
+  </si>
+  <si>
+    <t>PS.1.6</t>
+  </si>
+  <si>
+    <t>PS.1.7</t>
+  </si>
+  <si>
+    <t>PS.1.8</t>
+  </si>
+  <si>
+    <t>PS.1.9</t>
+  </si>
+  <si>
+    <t>PS.1.10</t>
+  </si>
+  <si>
+    <t>PS.1.11</t>
+  </si>
+  <si>
+    <t>PS.1.12</t>
+  </si>
+  <si>
+    <t>PS.1.13</t>
+  </si>
+  <si>
+    <t>PS.2.1</t>
+  </si>
+  <si>
+    <t>PS.2.2</t>
+  </si>
+  <si>
+    <t>PS.2.3</t>
+  </si>
+  <si>
+    <t>PS.2.4</t>
+  </si>
+  <si>
+    <t>PS.2.5</t>
+  </si>
+  <si>
+    <t>PS.2.6</t>
+  </si>
+  <si>
+    <t>PS.3.1</t>
+  </si>
+  <si>
+    <t>PS.3.2</t>
+  </si>
+  <si>
+    <t>PS.3.3</t>
+  </si>
+  <si>
+    <t>PS.3.4</t>
+  </si>
+  <si>
+    <t>PS.3.5</t>
+  </si>
+  <si>
+    <t>PS.3.6</t>
+  </si>
+  <si>
+    <t>PS.3.7</t>
+  </si>
+  <si>
+    <t>PS.3.8</t>
+  </si>
+  <si>
+    <t>PS.3.9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,15 +332,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C60201B-D876-4109-8647-FE7C1079C08C}" name="Table1" displayName="Table1" ref="B2:I3" totalsRowShown="0">
-  <autoFilter ref="B2:I3" xr:uid="{1C60201B-D876-4109-8647-FE7C1079C08C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C60201B-D876-4109-8647-FE7C1079C08C}" name="Table1" displayName="Table1" ref="B2:I40" totalsRowShown="0">
+  <autoFilter ref="B2:I40" xr:uid="{1C60201B-D876-4109-8647-FE7C1079C08C}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{61333736-D8AE-4E92-8083-E0CA1447312A}" name="Requirement"/>
     <tableColumn id="2" xr3:uid="{3BFEB35C-ED06-4F45-ABB0-1959FF28BE4A}" name="Subrequirement"/>
     <tableColumn id="3" xr3:uid="{31DCF9F4-D0AB-48D6-B273-6A61762E92FB}" name="User Requirement"/>
     <tableColumn id="4" xr3:uid="{F88B3A48-8665-40A1-B555-E18A8C57A7A1}" name="Solves"/>
     <tableColumn id="5" xr3:uid="{458E62CE-F2DB-43E8-A0B1-3AE1827047B4}" name="Evidence"/>
-    <tableColumn id="6" xr3:uid="{32E7F817-A24D-47CA-9E2F-56B731209DAA}" name="Justification"/>
+    <tableColumn id="6" xr3:uid="{32E7F817-A24D-47CA-9E2F-56B731209DAA}" name="Justification/Limitation"/>
     <tableColumn id="7" xr3:uid="{EA67DD74-0EA9-4894-93DB-334F56C81888}" name="Success Criteria"/>
     <tableColumn id="8" xr3:uid="{853CCA24-6CE7-472E-AF5E-76CD171E3972}" name="Github link to issues"/>
   </tableColumns>
@@ -404,29 +611,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I3"/>
+  <dimension ref="B2:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="4" max="4" width="31.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.44140625" customWidth="1"/>
     <col min="7" max="7" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -438,39 +646,405 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>